<commit_message>
Clean sheet names of disallowed characters
</commit_message>
<xml_diff>
--- a/test/files/autofilter.xlsx
+++ b/test/files/autofilter.xlsx
@@ -11,8 +11,8 @@
     <sheet name="sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">sheet1!$A$1:$J$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="1">sheet2!$A$1:$J$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="0">'sheet1'!$A$1:$J$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" hidden="1" localSheetId="1">'sheet2'!$A$1:$J$12</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>

</xml_diff>